<commit_message>
Update simulation to 010
</commit_message>
<xml_diff>
--- a/data/seir_simulation.xlsx
+++ b/data/seir_simulation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27975" windowHeight="12450"/>
+    <workbookView windowHeight="15800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>ID</t>
   </si>
@@ -151,8 +151,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -164,16 +164,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,15 +189,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,9 +210,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -225,13 +232,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -242,12 +265,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -255,54 +301,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,25 +323,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,67 +485,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,85 +503,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,6 +514,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -570,32 +585,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,153 +605,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -768,10 +768,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,39 +792,39 @@
     <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -953,7 +953,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -977,9 +977,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1003,7 +1003,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1056,7 +1056,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1081,7 +1081,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1091,23 +1091,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.8" style="1"/>
-    <col min="2" max="2" width="11" customWidth="true"/>
-    <col min="3" max="3" width="12.9" customWidth="true"/>
-    <col min="6" max="6" width="31.9" customWidth="true"/>
-    <col min="7" max="7" width="15.8" customWidth="true"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" customWidth="1"/>
+    <col min="6" max="6" width="31.8984375" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1460,9 +1460,39 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1.8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>43</v>
+      </c>
+      <c r="I11">
+        <v>0.5</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1000000</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
Update simulation to id 012
</commit_message>
<xml_diff>
--- a/data/seir_simulation.xlsx
+++ b/data/seir_simulation.xlsx
@@ -1098,7 +1098,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14"/>
@@ -1495,14 +1495,74 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>0.7</v>
+      </c>
+      <c r="D12">
+        <v>1.8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>43</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.8</v>
+      </c>
+      <c r="D13">
+        <v>1.8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>43</v>
+      </c>
+      <c r="I13">
+        <v>0.5</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1000000</v>
       </c>
     </row>
     <row r="14" spans="1:1">

</xml_diff>

<commit_message>
Update simulation to id 016
</commit_message>
<xml_diff>
--- a/data/seir_simulation.xlsx
+++ b/data/seir_simulation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15800"/>
+    <workbookView windowWidth="27975" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -150,10 +150,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -165,7 +165,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,8 +224,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -196,39 +280,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -241,60 +295,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -323,49 +323,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,49 +491,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,79 +503,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,17 +517,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,6 +546,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,30 +609,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -619,148 +619,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -768,10 +768,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,39 +792,39 @@
     <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
-    <cellStyle name="Total" xfId="24" builtinId="25"/>
-    <cellStyle name="Output" xfId="25" builtinId="21"/>
-    <cellStyle name="Currency" xfId="26" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="Note" xfId="28" builtinId="10"/>
-    <cellStyle name="Input" xfId="29" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Good" xfId="32" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="Title" xfId="38" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
-    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
-    <cellStyle name="Link" xfId="43" builtinId="8"/>
-    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
-    <cellStyle name="Comma" xfId="45" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -953,7 +953,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -977,9 +977,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1003,7 +1003,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1056,7 +1056,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1081,7 +1081,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1091,23 +1091,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.8984375" customWidth="1"/>
-    <col min="6" max="6" width="31.8984375" customWidth="1"/>
-    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="1" max="1" width="8.8" style="1"/>
+    <col min="2" max="2" width="11" customWidth="true"/>
+    <col min="3" max="3" width="12.9" customWidth="true"/>
+    <col min="6" max="6" width="31.9" customWidth="true"/>
+    <col min="7" max="7" width="15.8" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1565,24 +1565,144 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>0.9</v>
+      </c>
+      <c r="D14">
+        <v>1.8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>43</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>0.6</v>
+      </c>
+      <c r="D15">
+        <v>1.8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>43</v>
+      </c>
+      <c r="I15">
+        <v>0.5</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>1.8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.4</v>
+      </c>
+      <c r="D17">
+        <v>1.8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>43</v>
+      </c>
+      <c r="I17">
+        <v>0.5</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1000000</v>
       </c>
     </row>
     <row r="18" spans="1:1">

</xml_diff>

<commit_message>
Update to simulation to id 017
</commit_message>
<xml_diff>
--- a/data/seir_simulation.xlsx
+++ b/data/seir_simulation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -150,10 +150,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -164,6 +164,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -171,8 +179,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,15 +224,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -209,23 +248,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,68 +301,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -329,19 +329,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,85 +473,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,61 +485,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,15 +514,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -580,21 +571,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -614,153 +590,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1096,9 +1096,9 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
@@ -1705,9 +1705,39 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>0.3</v>
+      </c>
+      <c r="D18">
+        <v>1.8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>43</v>
+      </c>
+      <c r="I18">
+        <v>0.5</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1000000</v>
       </c>
     </row>
     <row r="19" spans="1:1">

</xml_diff>